<commit_message>
fix bugs of wildcard explanation and keyword searching
</commit_message>
<xml_diff>
--- a/download_table/uom_sign_links.xlsx
+++ b/download_table/uom_sign_links.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +437,1419 @@
     <col width="100" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>source_link</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>associated_text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-CCV-Grants-in-Aid-EOI-online-form-template-for-internal-use.docx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/cancer-council-victoria-grants-in-aid</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>internal UoM template</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25-Eligiblity-Exemption-Request-Form.xlsx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>here</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/NHMRC-2020-Presentation-18-March-2020-SL.pptx</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/university-of-melbourne-a*star-call-for-collaborative-phd-project-proposals/Outcomes-Joint-PhD-ASTAR.pdf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/university-of-melbourne-a*star-call-for-collaborative-phd-project-proposals</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>List of Projects</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2023-ECRF-MCRF-HeadofResearchTeam-Template.docx</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/vca-grants</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ECRF</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT_DECRA_EER-Info-Sheet_updated-20240904.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DE26 EER Info Sheet </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/UoM_confidential_Industry-Fellowship-Advice_Final_13July.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>UoM Industry Fellowship Guide (updated 14/07/23)</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25_RIC_C2_Template_v1.docx</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>DE25 C2 Administering Organisation Letter of Support Template</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25-UoM_Salary-Scales_Budget_021123_FINAL.xlsx</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>DE25 Salary Scales and Budget Preparation Spreadsheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25_RIC_Admin-Org-Support-Letter-Guide_v1.pdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>DE25 C2 Administering Organisation Letter of Support Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IM24-Research-Time-Calculator-amended.xlsx</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>IM24 Research Time Calculator</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25_UoM_authority_to_submit_form_v2.docx</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>DE25 Authority to Submit Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE26_Eligiblity-Exemption-Request-Form.xlsx</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>DE26 Eligibility Exemption Request (EER) Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IM24_UoM_authority_to_submit_form.docx</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>IM24 Authority to Submit Form (updated 12/07/2023)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/NIT-workshop-slides.pdf</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">slides </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DE25_RIC_appguide_v1.pdf</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>DE25 RIC Applicant Guide updated</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Industry-Fellowship-outcomes-analysis_Final.pptx</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2020-08-12,-GaRDeN-2-ROPE-1-vFINALset.pdf</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC_FT24_DE25_Information_Seminar_Q-and-A_19102023.pdf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Q&amp;A</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-DECRA23-Info-Webinar-Budgets-FINAL.pdf</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-FDP-Budget-Slides-22-09-2020.pdf</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/rope-1-presenting-your-career-journey-august-2020</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/mid-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-ARC-COE-FOR-division-updated-20240123.xlsx</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2024 ARC College of Experts Members - FOR division</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC-Rejoinder-Fact-Sheet_March-2022.pdf</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>UoM Rejoinder fact sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-DE23-Rejoinders_RIC_FINAL.pdf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>DE23 DECRA Rejoinder Webinar Slide</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-DECRA24-Info-Webinar_-FINAL.pdf</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/decra</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/toronto-melbourne-irtg-call-for-proposals/Outcomes,-Joint-PhD-Toronto-Melbourne-2024.pdf</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/toronto-melbourne-irtg-call-for-proposals</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Projects Awarded</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/UoM-Co-Investment-Request-Form_2024-VDOH-VMRAF_updated-21-Nov-23.docx</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/djpr-victorian-medical-research-acceleration-fund-vmraf-and-mrna-vmraf</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Cash Co-Investment Request Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-VMRAF-R7-DVCR-Lead-Letter-of-Support-template.docx</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/djpr-victorian-medical-research-acceleration-fund-vmraf-and-mrna-vmraf</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>DVCR Letter of Support template</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/national-institutes-of-health-scheme/national-institutes-of-health/propsal-development-resources</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/national-institutes-of-health-scheme</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Proposal Development Resources</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2025_Westpac_Eligibility-Exemption-Request-Calculator_V2.xlsx</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/westpac</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Eligibility Exemption Calculator</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship/IE24-Frequently-Asked-Questions.pdf</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>IE24 Frequently Asked Questions V1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IE24-Research-Time-Calculator.xlsx</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>IE24 Research Time Calculator</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IE24_UoM_authority_to_submit_form_15082023.docx</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>IE24 Authority to Submit form</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship/Industry-Fellowship-outcomes-analysis_Edit_SV14Sept.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slides </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC_IN25_Authority-to-Submit-Form.docx</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>IN25 RIC Authority to Submit Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IN25-Part-B3-Research-Load-Template.docx</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>IN25 Part B3 Research Load Template</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/IN25-UoM_Salary-Scales_Budget_V2.xlsx</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>IN25 Salary Scales and Budget Preparation</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-ARC-COE-FOR-division.xlsx</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2024 College of Experts Members - FOR division</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/UoM-Co-Investment-Request-Form_2024-DJSIR-mRNA-VRAF_updated-21-Nov-23.docx</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/mrna-vraf-round-3</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Cash Co-Investment Request Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DP25-Salary-Scales-and-Budget-Preparation_v1_090424.xlsx</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>DP25 Salary Scales and Budget Preparation Tool</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DP25_Applicant_Guide_V2.pdf</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>DP25 RIC Applicant Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-mRNA-VRAF-R3-DVCR-Lead-Letter-of-Support-template.docx</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/mrna-vraf-round-3</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>DVCR Letter of Support template</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC_DPEI25_Top_Ten_Tips_Final_Submission_16022024.pdf</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>DP25 EOI Top Ten Tips for Final Submission</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DPEOI_25_Applicant_Guide_V4.pdf</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>DP25 EOI RIC Applicant Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DPEOI25_Advice-for-PIs_V2.docx</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>DP25 EOI RIC Advice for PIs</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-DP25-Full-Application-Stage_Seminar_17042024.pdf</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC_CRE_Seminar_Advice-for-ARC-DP-ROPE_19022024_slides.pdf</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ARC-DP25-Major-Changes.pdf</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">slides </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/How-to-Pitch-an-EOI-combined-slides.pdf</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DP25-ROPE-Seminar-Q-and-A_19022024.pdf</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Q&amp;A</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DP24-RIC-Discovery-Projects-Seminar.pdf</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DARPA-and-IARPA-FAQs.pdf</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/department-of-defense-dod/dod-agencies</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>DARPA &amp; IARPA FAQs</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DP23-webinar_Final.pdf</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-projects</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DARPA-Workshop_FINAL.pdf</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/department-of-defense-dod/dod-agencies</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Preparing and Submitting USA Dept of Defense Applications</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/DRAFT-FT25_Eligiblity-Exemption-Request-Form.xlsx</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>here</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25_UoM_authority_to_submit_form_final.docx</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>FT25 Authority to Submit form</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25_Eligiblity-Exemption-Request-Form.xlsx</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>FT25 Eligibility Exemption Request (EER) Form</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Slides-3-Workshop-1-JOD-overheads-v2.pdf</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Slides3</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/is-an-arc-fellowship-right-for-you-28-july-2020</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/crafting-a-well-justified-arc-fellowship-budget-22-sept-2020</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25-Part-B4-Research-Load-Table-Template-final.docx</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>FT25 Part B4 Research Load Template</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25_RIC_Admin-Org-Support-Letter-Guide-final.pdf</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>FT25 C2 Administering Organisation Letter of Support guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25_RIC_C2_Template_final.docx</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>FT25 C2 Administering Organisation Letter of Support template</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25-UoM_Salary-Scales-and-Budget-Preparation.xlsx</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Salary Scales and Budget Preparation Spreadsheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Slides1-Is-an-ARC-Fellowship-right-for-you-Kate-Smith-Miles.pdf</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Slides1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/FT25-RIC-Info-Webinar-combined.pdf</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Slides </t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/LP24-Part-B3-Research-Load-Template.docx</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>LP24 Research Load Template (Part B3)</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC-ARC-FT-DECRA-webinar-slides.pdf</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC-ARC-FT-DECRA-webinar-additional-questions.pdf</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Additional Q&amp;A</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/LP24_Salary-Scales-and-Budget-Preparation.xlsx</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LP24 Salary Scales and Budget Preparation Spreadsheet </t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Linkage-Projects-Factsheet-Pre-Award_2023_Final.pdf</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Linkage Projects Factsheet - Pre Award</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2024-Linkage-Webinar-Navigating-the-process.pptx</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/RIC_UnveilingLinkageSuccess_slides.pptx</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects/2023-RIC-Linkage-Webinar-Final_4-Oct.pdf</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/2023-RIC-Linkage-Webinar-Final.pptx</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>slides</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/LP24_Applicant_Guide_V2.pdf</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>LP24 RIC Applicant Guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Slides2-Presentation_2020July28_Recalde_revised.pdf</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Slides2</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/LP23_Partner-Investigator-Info-Booklet_Draft_EM_SV_Final_9Mar23.docx</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Partner Investigators information booklet – Include sample letter, RMS details, scheme information</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/Linkage-Agreements-Factsheet-Post-Award_2023_Final.pdf</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Linkage Agreements Factsheet - Post Award</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/ric-arc-ft-decra-webinar-15-october-2020</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/future-fellowships</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/assets/interim-private-files/LP24_Authority-to-Submit_R2_v2.docx</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/linkage-projects</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>LP24 Authority to Submit form</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>